<commit_message>
2nd Commit with Completing all the scenarios and validation with running on IE, chrome and firefox.
</commit_message>
<xml_diff>
--- a/AtmecsAutomation/src/test/resources/testData/testinput.xlsx
+++ b/AtmecsAutomation/src/test/resources/testData/testinput.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15570" windowHeight="5880" tabRatio="544" firstSheet="1" activeTab="2"/>
+    <workbookView windowWidth="15570" windowHeight="5880" tabRatio="544" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
@@ -46,18 +46,18 @@
     <t>Artificial Intelligence / Machine Learning</t>
   </si>
   <si>
+    <t>Augmented Reality / Virtual Reality</t>
+  </si>
+  <si>
+    <t>Internet of Things</t>
+  </si>
+  <si>
     <t>Blockchain</t>
   </si>
   <si>
-    <t>Augmented Reality / Virtual Reality</t>
-  </si>
-  <si>
     <t>Robotic Process Automation &amp; ChatBOTs</t>
   </si>
   <si>
-    <t>Internet of Things</t>
-  </si>
-  <si>
     <t>Infrastructure Management</t>
   </si>
   <si>
@@ -112,13 +112,13 @@
     <t>info@atmecs.com</t>
   </si>
   <si>
+    <t>Cloud Services</t>
+  </si>
+  <si>
+    <t>Enterprise Analytics</t>
+  </si>
+  <si>
     <t>Quality Engineering</t>
-  </si>
-  <si>
-    <t>Cloud Services</t>
-  </si>
-  <si>
-    <t>Enterprise Analytics</t>
   </si>
   <si>
     <t>Mobile Computing</t>
@@ -132,10 +132,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -146,9 +146,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -162,6 +176,112 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -169,126 +289,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -299,19 +299,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -329,25 +425,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -359,7 +443,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -371,115 +479,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,26 +493,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -532,17 +532,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -554,15 +557,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -582,11 +576,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -595,15 +595,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -613,130 +613,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1119,36 +1119,40 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:B4"/>
+  <dimension ref="A2:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="1" width="44.8571428571429" customWidth="1"/>
     <col min="2" max="2" width="36.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1163,7 +1167,7 @@
   <sheetPr/>
   <dimension ref="A2:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
@@ -1336,64 +1340,55 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A4:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:A10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="39.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="21.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
+      <c r="B8" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit with completing the scenarios and validation with proper comments and grid configuration
</commit_message>
<xml_diff>
--- a/AtmecsAutomation/src/test/resources/testData/testinput.xlsx
+++ b/AtmecsAutomation/src/test/resources/testData/testinput.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15570" windowHeight="5880" tabRatio="544" firstSheet="2" activeTab="5"/>
+    <workbookView windowWidth="14265" windowHeight="4890" tabRatio="544" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
@@ -132,9 +132,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
@@ -146,25 +146,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -177,7 +170,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -191,35 +191,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -227,33 +199,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,26 +246,47 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -299,13 +299,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -317,61 +425,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -383,49 +449,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,49 +479,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -497,46 +497,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -545,17 +506,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -576,6 +526,47 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -590,20 +581,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -613,130 +613,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1168,7 +1168,7 @@
   <dimension ref="A2:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
@@ -1252,7 +1252,7 @@
   <sheetPr/>
   <dimension ref="A2:A15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:A15"/>
     </sheetView>
   </sheetViews>
@@ -1342,8 +1342,8 @@
   <sheetPr/>
   <dimension ref="A4:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B8"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="1"/>

</xml_diff>